<commit_message>
Upgrade CM to support AnyInfo mode
</commit_message>
<xml_diff>
--- a/CM.xlsx
+++ b/CM.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="95">
   <si>
     <t>Funcoes:</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Size = 7 bytes (sem start/end)</t>
   </si>
   <si>
-    <t>ERROR</t>
-  </si>
-  <si>
     <t>0xFF</t>
   </si>
   <si>
@@ -254,12 +251,6 @@
     <t>00 00~03 ff</t>
   </si>
   <si>
-    <t>0x20</t>
-  </si>
-  <si>
-    <t>Input Error</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
@@ -288,6 +279,39 @@
   </si>
   <si>
     <t>light +</t>
+  </si>
+  <si>
+    <t>Read Any info</t>
+  </si>
+  <si>
+    <t>0x30</t>
+  </si>
+  <si>
+    <t>10 ~ 18</t>
+  </si>
+  <si>
+    <t>0x18</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>0x19</t>
+  </si>
+  <si>
+    <t>RESERVED</t>
+  </si>
+  <si>
+    <t>0xEX</t>
+  </si>
+  <si>
+    <t>00 00~ff fe</t>
+  </si>
+  <si>
+    <t>Fail to measure</t>
+  </si>
+  <si>
+    <t>PriorityMsg</t>
   </si>
 </sst>
 </file>
@@ -343,7 +367,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -403,11 +427,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -457,25 +503,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -496,7 +536,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2063,10 +2124,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S29"/>
+  <dimension ref="B1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,20 +2155,20 @@
       <c r="E2" s="5"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="L2" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
     </row>
     <row r="3" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
@@ -2116,26 +2177,26 @@
       <c r="E3" s="5"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="34"/>
-      <c r="J3" s="35"/>
-      <c r="L3" s="29" t="s">
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
+      <c r="L3" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
     </row>
     <row r="4" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="28"/>
       <c r="F4" s="17" t="s">
         <v>63</v>
       </c>
@@ -2149,22 +2210,22 @@
       <c r="J4" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="26" t="s">
+      <c r="L4" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="28" t="s">
+      <c r="M4" s="37"/>
+      <c r="N4" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28" t="s">
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="R4" s="28"/>
+      <c r="R4" s="25"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="29" t="s">
         <v>52</v>
       </c>
       <c r="D5" s="12" t="s">
@@ -2207,7 +2268,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="31"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="12" t="s">
         <v>53</v>
       </c>
@@ -2219,7 +2280,7 @@
         <v>67</v>
       </c>
       <c r="I6" s="6" t="str">
-        <f t="shared" ref="I6:I26" si="1">CONCATENATE("0x",DEC2HEX(F6,2))</f>
+        <f t="shared" ref="I6:I24" si="1">CONCATENATE("0x",DEC2HEX(F6,2))</f>
         <v>0x01</v>
       </c>
       <c r="J6" s="6" t="s">
@@ -2249,7 +2310,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="31"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="12" t="s">
         <v>27</v>
       </c>
@@ -2290,7 +2351,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="31"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="12" t="s">
         <v>54</v>
       </c>
@@ -2331,7 +2392,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="31"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="12" t="s">
         <v>33</v>
       </c>
@@ -2372,7 +2433,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="31"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="12" t="s">
         <v>55</v>
       </c>
@@ -2413,7 +2474,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="31"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="12" t="s">
         <v>56</v>
       </c>
@@ -2454,7 +2515,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="31"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="12" t="s">
         <v>57</v>
       </c>
@@ -2495,7 +2556,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C13" s="31"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="12" t="s">
         <v>24</v>
       </c>
@@ -2551,11 +2612,11 @@
       <c r="R14" s="6"/>
     </row>
     <row r="15" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="32" t="s">
-        <v>77</v>
+      <c r="C15" s="30" t="s">
+        <v>74</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F15" s="6">
         <v>16</v>
@@ -2577,13 +2638,13 @@
         <v>67</v>
       </c>
       <c r="N15" s="6" t="str">
-        <f t="shared" ref="N15:N26" si="2">I15</f>
+        <f t="shared" ref="N15:N27" si="2">I15</f>
         <v>0x10</v>
       </c>
-      <c r="O15" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P15" s="22"/>
+      <c r="O15" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="P15" s="27"/>
       <c r="Q15" s="6" t="s">
         <v>66</v>
       </c>
@@ -2592,9 +2653,9 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="32"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F16" s="6">
         <v>17</v>
@@ -2620,10 +2681,10 @@
         <f t="shared" si="2"/>
         <v>0x11</v>
       </c>
-      <c r="O16" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P16" s="22"/>
+      <c r="O16" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="P16" s="27"/>
       <c r="Q16" s="6" t="s">
         <v>66</v>
       </c>
@@ -2632,9 +2693,9 @@
       </c>
     </row>
     <row r="17" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C17" s="32"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F17" s="6">
         <v>18</v>
@@ -2659,10 +2720,10 @@
         <f t="shared" si="2"/>
         <v>0x12</v>
       </c>
-      <c r="O17" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P17" s="22"/>
+      <c r="O17" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="P17" s="27"/>
       <c r="Q17" s="6" t="s">
         <v>66</v>
       </c>
@@ -2671,7 +2732,7 @@
       </c>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C18" s="32"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="12"/>
       <c r="F18" s="6"/>
       <c r="H18" s="6"/>
@@ -2687,9 +2748,9 @@
       <c r="S18" s="10"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C19" s="32"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F19" s="6">
         <v>19</v>
@@ -2714,10 +2775,10 @@
         <f t="shared" ref="N19:N21" si="3">I19</f>
         <v>0x13</v>
       </c>
-      <c r="O19" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P19" s="22"/>
+      <c r="O19" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="P19" s="27"/>
       <c r="Q19" s="6" t="s">
         <v>66</v>
       </c>
@@ -2726,9 +2787,9 @@
       </c>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C20" s="32"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F20" s="6">
         <v>20</v>
@@ -2753,10 +2814,10 @@
         <f t="shared" si="3"/>
         <v>0x14</v>
       </c>
-      <c r="O20" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P20" s="22"/>
+      <c r="O20" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="P20" s="27"/>
       <c r="Q20" s="6" t="s">
         <v>66</v>
       </c>
@@ -2765,9 +2826,9 @@
       </c>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C21" s="32"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F21" s="6">
         <v>21</v>
@@ -2792,10 +2853,10 @@
         <f t="shared" si="3"/>
         <v>0x15</v>
       </c>
-      <c r="O21" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P21" s="22"/>
+      <c r="O21" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="P21" s="27"/>
       <c r="Q21" s="6" t="s">
         <v>66</v>
       </c>
@@ -2804,7 +2865,7 @@
       </c>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C22" s="32"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="12"/>
       <c r="F22" s="6"/>
       <c r="H22" s="6"/>
@@ -2819,9 +2880,9 @@
       <c r="R22" s="6"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C23" s="32"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F23" s="6">
         <v>22</v>
@@ -2842,14 +2903,13 @@
       <c r="M23" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="N23" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>0x16</v>
-      </c>
-      <c r="O23" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P23" s="22"/>
+      <c r="N23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O23" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="P23" s="27"/>
       <c r="Q23" s="6" t="s">
         <v>66</v>
       </c>
@@ -2858,9 +2918,9 @@
       </c>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C24" s="32"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F24" s="6">
         <v>23</v>
@@ -2881,156 +2941,229 @@
       <c r="M24" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="N24" s="36" t="str">
+      <c r="N24" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O24" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C25" s="30"/>
+      <c r="D25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="6">
+        <v>24</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N25" s="12" t="str">
+        <f t="shared" ref="N25" si="4">I25</f>
+        <v>0x18</v>
+      </c>
+      <c r="O25" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="R25" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C26" s="30"/>
+      <c r="D26" s="12"/>
+      <c r="F26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+    </row>
+    <row r="27" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C27" s="30"/>
+      <c r="D27" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="6">
+        <v>24</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N27" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>0x17</v>
-      </c>
-      <c r="O24" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="R24" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="32"/>
-      <c r="D25" s="12"/>
-      <c r="F25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="21"/>
-      <c r="P25" s="21"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-    </row>
-    <row r="26" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C26" s="32"/>
-      <c r="D26" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="6">
-        <v>24</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="I26" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>0x18</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N26" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>0x18</v>
-      </c>
-      <c r="O26" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="R26" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C28" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="25"/>
-      <c r="H28" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N28" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="O28" s="6" t="s">
+        <v>0x19</v>
+      </c>
+      <c r="O27" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="R27" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C29" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="35"/>
+      <c r="H29" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="O29" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="R29" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C30" s="23"/>
+      <c r="D30" s="24"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+    </row>
+    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C31" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+    </row>
+    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C32" s="43"/>
+      <c r="D32" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="L32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N32" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="P28" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="R28" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C29" s="23" t="s">
+      <c r="O32" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="23"/>
-      <c r="H29" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="I29" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="J29" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="O29" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="P29" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q29" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="R29" s="6" t="s">
+      <c r="P32" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q32" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="R32" s="6" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="23">
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="C31:C32"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="L2:R2"/>
     <mergeCell ref="L3:R3"/>
-    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O27:P27"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:C13"/>
-    <mergeCell ref="C15:C26"/>
+    <mergeCell ref="C15:C27"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="H3:J3"/>
@@ -3040,11 +3173,6 @@
     <mergeCell ref="O19:P19"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="L4:M4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>